<commit_message>
Uploading final files, Jupyter Notebook and SQL code.
</commit_message>
<xml_diff>
--- a/EmployeeSQL/all_files_details.xlsx
+++ b/EmployeeSQL/all_files_details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando\Desktop\sql-challenge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando\Desktop\sql-challenge\EmployeeSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996E86DE-C57A-407A-8423-AB42C5920320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AB8CAC-818C-4076-88ED-2B195C7641F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F524264F-C697-4E64-894F-B22E52F7F86B}"/>
   </bookViews>
@@ -24,7 +24,6 @@
     <sheet name="Task 8" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="88">
   <si>
     <t>departments.csv</t>
   </si>
@@ -250,12 +249,6 @@
   </si>
   <si>
     <t>All files details'</t>
-  </si>
-  <si>
-    <t>LEFT</t>
-  </si>
-  <si>
-    <t>RIGHT</t>
   </si>
   <si>
     <t xml:space="preserve">TASK 1   </t>
@@ -341,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,12 +362,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -489,6 +476,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -507,11 +498,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,6 +854,7 @@
       <c r="J4" s="8"/>
       <c r="N4" s="8"/>
       <c r="W4" s="8"/>
+      <c r="AA4" s="8"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -1556,12 +1543,12 @@
       <c r="L18" s="3">
         <v>110386</v>
       </c>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="D19" s="10"/>
+      <c r="K19" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1591,44 +1578,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>74</v>
+      <c r="A2" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="B3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="6" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -1680,34 +1660,34 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="6" t="s">
+    <row r="10" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="6" t="s">
+      <c r="L10" s="12"/>
+      <c r="M10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="12" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1997,38 +1977,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>76</v>
+      <c r="A2" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="B3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="8"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
@@ -2066,27 +2046,27 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="6" t="s">
+    <row r="10" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="12" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2328,37 +2308,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>78</v>
+      <c r="A2" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="B3" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="6" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="6" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -2425,41 +2405,41 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="6" t="s">
+    <row r="10" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="5" t="s">
+      <c r="L10" s="12"/>
+      <c r="M10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="5" t="s">
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="R10" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2847,37 +2827,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>80</v>
+      <c r="A2" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="B3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="6" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="6" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -2944,41 +2924,41 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="6" t="s">
+    <row r="10" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="5" t="s">
+      <c r="L10" s="12"/>
+      <c r="M10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="5" t="s">
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="R10" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3359,37 +3339,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>82</v>
+      <c r="A2" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="B3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="6" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="6" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -3426,27 +3406,27 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="6" t="s">
+    <row r="10" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="12" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3693,37 +3673,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>85</v>
+      <c r="A2" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="B3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="6" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="6" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -3790,41 +3770,41 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="18" t="s">
+    <row r="10" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="5" t="s">
+      <c r="L10" s="12"/>
+      <c r="M10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="19" t="s">
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="R10" s="12" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4209,37 +4189,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>86</v>
+      <c r="A2" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="B3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="6" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="6" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -4306,41 +4286,41 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="19"/>
-      <c r="D10" s="7" t="s">
+    <row r="10" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19" t="s">
+      <c r="L10" s="12"/>
+      <c r="M10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19" t="s">
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="19" t="s">
+      <c r="R10" s="12" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4725,37 +4705,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>89</v>
+      <c r="A2" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="B3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="6" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="6" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -4822,41 +4802,41 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="18" t="s">
+    <row r="10" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="5" t="s">
+      <c r="L10" s="12"/>
+      <c r="M10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="19" t="s">
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="R10" s="12" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>